<commit_message>
Correction of Formula linkage.
</commit_message>
<xml_diff>
--- a/rpt/nested.xlsx
+++ b/rpt/nested.xlsx
@@ -77,6 +77,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="C11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Name</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D10" authorId="0">
       <text>
         <r>
@@ -90,6 +103,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Description</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E10" authorId="0">
       <text>
         <r>
@@ -103,6 +129,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">RecipeQty</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F6" authorId="0">
       <text>
         <r>
@@ -142,6 +181,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="F11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Quantity</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H10" authorId="0">
       <text>
         <r>
@@ -155,7 +207,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Price</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t xml:space="preserve">Inventory Report Category with Sub-Category</t>
   </si>
@@ -239,6 +317,9 @@
   </si>
   <si>
     <t xml:space="preserve">NANGKA SAYUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~Item.BoM:A</t>
   </si>
   <si>
     <t xml:space="preserve">~Item.BoM:F</t>
@@ -251,9 +332,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0.00;[RED]\([$Rp-421]#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -320,12 +402,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -361,7 +450,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,19 +479,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,10 +580,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -608,47 +705,75 @@
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="10" t="n">
         <f aca="false">F10/E10</f>
         <v>2</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="I10" s="9" t="n">
+      <c r="I10" s="11" t="n">
         <v>1500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>100</v>
+      </c>
       <c r="G11" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="10" t="s">
+        <f aca="false">F11/E11</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>2</v>
+      <c r="G12" s="12" t="n">
+        <f aca="false">MIN(G10:G11)</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CostValue, plus its digits
</commit_message>
<xml_diff>
--- a/rpt/nested.xlsx
+++ b/rpt/nested.xlsx
@@ -596,8 +596,8 @@
   </sheetPr>
   <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -727,14 +727,14 @@
         <v>21</v>
       </c>
       <c r="F10" s="10" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G10" s="10" t="n">
         <v>100</v>
       </c>
       <c r="H10" s="10" t="n">
         <f aca="false">G10/F10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10" s="11" t="n">
         <v>30</v>
@@ -774,9 +774,9 @@
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="14" t="n">
-        <f aca="false">MIN(H10:H11)</f>
-        <v>2</v>
+      <c r="H12" s="14" t="e">
+        <f aca="false">MIN(H10:h[1]Sheet!G8711)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
bugfix error logic: wrong getting parent state. solved by saving current data in fxl
</commit_message>
<xml_diff>
--- a/rpt/nested.xlsx
+++ b/rpt/nested.xlsx
@@ -388,7 +388,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -596,14 +596,14 @@
   </sheetPr>
   <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.11"/>
@@ -770,13 +770,13 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="14" t="e">
-        <f aca="false">MIN(H10:h[1]Sheet!G8711)</f>
-        <v>#VALUE!</v>
+      <c r="H12" s="14" t="n">
+        <f aca="false">MIN(H10:H11)</f>
+        <v>2</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
BUGFIX footer formula bugfix formula range in footer, +mute console +costs source field name.
</commit_message>
<xml_diff>
--- a/rpt/nested.xlsx
+++ b/rpt/nested.xlsx
@@ -168,6 +168,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Value</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G10" authorId="0">
       <text>
         <r>
@@ -203,37 +216,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Price</t>
+          <t xml:space="preserve">Value</t>
         </r>
       </text>
     </comment>
     <comment ref="I11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Price</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Value</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">Inventory Report Category with Sub-Category</t>
   </si>
@@ -289,6 +276,9 @@
     <t xml:space="preserve">RECIPE</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Item</t>
   </si>
   <si>
@@ -307,7 +297,7 @@
     <t xml:space="preserve">Unit Cost</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost Value</t>
+    <t xml:space="preserve">Cost</t>
   </si>
   <si>
     <t xml:space="preserve">~Item.BoM</t>
@@ -320,6 +310,9 @@
   </si>
   <si>
     <t xml:space="preserve">~Item.BoM:A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KECAP MANIS BANGO (6.2 Kg)</t>
   </si>
   <si>
     <t xml:space="preserve">~Item.BoM:F</t>
@@ -335,7 +328,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0.00;[RED]\([$Rp-421]#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -456,7 +449,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,27 +478,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,6 +527,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -597,7 +618,7 @@
   <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,8 +631,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
@@ -689,97 +710,109 @@
       <c r="D8" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>12855.5333</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="G10" s="10" t="n">
+      <c r="G10" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="12" t="n">
         <f aca="false">G10/F10</f>
         <v>5</v>
       </c>
-      <c r="I10" s="11" t="n">
+      <c r="I10" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="J10" s="11" t="n">
-        <v>1500</v>
+      <c r="J10" s="13" t="n">
+        <f aca="false">I10*F10</f>
+        <v>600</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="G11" s="12" t="n">
+      <c r="E11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="17" t="n">
         <f aca="false">G11/F11</f>
-        <v>2</v>
-      </c>
-      <c r="I11" s="13" t="n">
+        <v>500</v>
+      </c>
+      <c r="I11" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="J11" s="13" t="n">
-        <v>1500</v>
+      <c r="J11" s="18" t="n">
+        <f aca="false">I11*F11</f>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="14" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" s="19" t="n">
         <f aca="false">MIN(H10:H11)</f>
-        <v>2</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>24</v>
+        <v>5</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="21" t="n">
+        <f aca="false">SUM(J10:J11)</f>
+        <v>606</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>